<commit_message>
Update bitcoin_buys.xlsx after running on 2025-05-04
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -1,66 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding_stuff\crypto_buys\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1432B0ED-62E9-4E47-82AD-F33D9D7DA273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Coins</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>04/27/2025</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,45 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -401,170 +424,196 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Coins</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>45743</v>
       </c>
-      <c r="B2">
-        <v>4.8000000000000001E-5</v>
-      </c>
-      <c r="C2">
-        <v>88296.54</v>
-      </c>
-      <c r="D2">
-        <v>4.3499999999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="B2" t="n">
+        <v>4.8e-05</v>
+      </c>
+      <c r="C2" t="n">
+        <v>88296.53999999999</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4.35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
         <v>45744</v>
       </c>
-      <c r="B3">
-        <v>5.7569999999999995E-4</v>
-      </c>
-      <c r="C3">
-        <v>84738.99</v>
-      </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="B3" t="n">
+        <v>0.0005757</v>
+      </c>
+      <c r="C3" t="n">
+        <v>84738.99000000001</v>
+      </c>
+      <c r="D3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
         <v>45747</v>
       </c>
-      <c r="B4">
-        <v>5.842E-4</v>
-      </c>
-      <c r="C4">
-        <v>84745.15</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="B4" t="n">
+        <v>0.0005842</v>
+      </c>
+      <c r="C4" t="n">
+        <v>84745.14999999999</v>
+      </c>
+      <c r="D4" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
         <v>45747</v>
       </c>
-      <c r="B5">
-        <v>5.8379999999999999E-4</v>
-      </c>
-      <c r="C5">
+      <c r="B5" t="n">
+        <v>0.0005838</v>
+      </c>
+      <c r="C5" t="n">
         <v>84801.3</v>
       </c>
-      <c r="D5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="D5" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>45751</v>
       </c>
-      <c r="B6">
-        <v>5.7280000000000005E-4</v>
-      </c>
-      <c r="C6">
+      <c r="B6" t="n">
+        <v>0.0005728</v>
+      </c>
+      <c r="C6" t="n">
         <v>85157.64</v>
       </c>
-      <c r="D6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="D6" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
         <v>45752</v>
       </c>
-      <c r="B7">
-        <v>5.9100000000000005E-4</v>
-      </c>
-      <c r="C7">
+      <c r="B7" t="n">
+        <v>0.0005910000000000001</v>
+      </c>
+      <c r="C7" t="n">
         <v>83764.73</v>
       </c>
-      <c r="D7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="D7" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
         <v>45760</v>
       </c>
-      <c r="B8">
-        <v>5.8739999999999997E-4</v>
-      </c>
-      <c r="C8">
+      <c r="B8" t="n">
+        <v>0.0005874</v>
+      </c>
+      <c r="C8" t="n">
         <v>85117.37</v>
       </c>
-      <c r="D8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="D8" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
         <v>45766</v>
       </c>
-      <c r="B9">
-        <v>5.842E-4</v>
-      </c>
-      <c r="C9">
-        <v>85584.9</v>
-      </c>
-      <c r="D9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>5.2950000000000002E-4</v>
-      </c>
-      <c r="C10">
-        <v>94430.1</v>
-      </c>
-      <c r="D10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="B9" t="n">
+        <v>0.0005842</v>
+      </c>
+      <c r="C9" t="n">
+        <v>85584.89999999999</v>
+      </c>
+      <c r="D9" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>04/27/2025</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0005295</v>
+      </c>
+      <c r="C10" t="n">
+        <v>94430.10000000001</v>
+      </c>
+      <c r="D10" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
         <v>45777</v>
       </c>
-      <c r="B11">
-        <v>5.287E-4</v>
-      </c>
-      <c r="C11">
-        <v>94573.82</v>
-      </c>
-      <c r="D11">
+      <c r="B11" t="n">
+        <v>0.0005287</v>
+      </c>
+      <c r="C11" t="n">
+        <v>94573.82000000001</v>
+      </c>
+      <c r="D11" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>05/04/2025</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.0005185599999999995</v>
+      </c>
+      <c r="C12" t="n">
+        <v>96420.85775995073</v>
+      </c>
+      <c r="D12" t="n">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-05-07
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,6 +617,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05/07/2025</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0005152999999999998</v>
+      </c>
+      <c r="C13" t="n">
+        <v>97030.85581214831</v>
+      </c>
+      <c r="D13" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-05-11
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,6 +633,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>05/11/2025</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0004785600000000003</v>
+      </c>
+      <c r="C14" t="n">
+        <v>104480.1069876295</v>
+      </c>
+      <c r="D14" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-05-14
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,6 +649,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>05/14/2025</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.00048211</v>
+      </c>
+      <c r="C15" t="n">
+        <v>103710.7714007177</v>
+      </c>
+      <c r="D15" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-05-18
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,6 +665,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>05/18/2025</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.00048095</v>
+      </c>
+      <c r="C16" t="n">
+        <v>103960.9106975777</v>
+      </c>
+      <c r="D16" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-05-21
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -681,6 +681,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>05/21/2025</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0004661999999999999</v>
+      </c>
+      <c r="C17" t="n">
+        <v>107250.1072501073</v>
+      </c>
+      <c r="D17" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-05-25
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -697,6 +697,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>05/25/2025</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.0004602700000000005</v>
+      </c>
+      <c r="C18" t="n">
+        <v>108631.8899776217</v>
+      </c>
+      <c r="D18" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-05-28
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -713,6 +713,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>05/28/2025</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.0004615799999999996</v>
+      </c>
+      <c r="C19" t="n">
+        <v>108323.5842107545</v>
+      </c>
+      <c r="D19" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-06-04
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -729,6 +729,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>06/04/2025</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.0004723999999999996</v>
+      </c>
+      <c r="C20" t="n">
+        <v>104784.081287045</v>
+      </c>
+      <c r="D20" t="n">
+        <v>49.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-06-08
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,6 +745,22 @@
         <v>49.5</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>06/08/2025</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.00047116</v>
+      </c>
+      <c r="C21" t="n">
+        <v>105059.8522794804</v>
+      </c>
+      <c r="D21" t="n">
+        <v>49.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-06-11
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -761,6 +761,22 @@
         <v>49.5</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>06/11/2025</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.0004524999999999998</v>
+      </c>
+      <c r="C22" t="n">
+        <v>109392.2651933702</v>
+      </c>
+      <c r="D22" t="n">
+        <v>49.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-06-15
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -777,6 +777,22 @@
         <v>49.5</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>06/15/2025</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.0004702200000000004</v>
+      </c>
+      <c r="C23" t="n">
+        <v>106333.2057334864</v>
+      </c>
+      <c r="D23" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-06-18
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,6 +793,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>06/18/2025</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.0004780300000000008</v>
+      </c>
+      <c r="C24" t="n">
+        <v>104595.9458611382</v>
+      </c>
+      <c r="D24" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-06-22
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,6 +809,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>06/22/2025</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.0004844799999999989</v>
+      </c>
+      <c r="C25" t="n">
+        <v>103203.4346103041</v>
+      </c>
+      <c r="D25" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-06-25
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -825,6 +825,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>06/25/2025</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.0004631500000000007</v>
+      </c>
+      <c r="C26" t="n">
+        <v>107956.3856202093</v>
+      </c>
+      <c r="D26" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-06-29
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -841,6 +841,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>06/29/2025</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.0004638799999999998</v>
+      </c>
+      <c r="C27" t="n">
+        <v>107786.4965077175</v>
+      </c>
+      <c r="D27" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-07-02
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -857,6 +857,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>07/02/2025</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>-0.01231811</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-4059.064255798982</v>
+      </c>
+      <c r="D28" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-07-16
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -917,6 +917,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>07/16/2025</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.0004174600000000014</v>
+      </c>
+      <c r="C32" t="n">
+        <v>119771.9541992043</v>
+      </c>
+      <c r="D32" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-07-20
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -933,6 +933,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>07/20/2025</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.0004220200000000004</v>
+      </c>
+      <c r="C33" t="n">
+        <v>118477.7972607932</v>
+      </c>
+      <c r="D33" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-07-23
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -949,6 +949,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>07/23/2025</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.0004208400000000022</v>
+      </c>
+      <c r="C34" t="n">
+        <v>118809.9990495194</v>
+      </c>
+      <c r="D34" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-07-27
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -965,6 +965,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>07/27/2025</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.0004206000000000001</v>
+      </c>
+      <c r="C35" t="n">
+        <v>118877.7936281502</v>
+      </c>
+      <c r="D35" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-07-30
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -981,6 +981,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>07/30/2025</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.000422829999999999</v>
+      </c>
+      <c r="C36" t="n">
+        <v>118250.8336683776</v>
+      </c>
+      <c r="D36" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-08-03
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -997,6 +997,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>08/03/2025</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.0004380899999999986</v>
+      </c>
+      <c r="C37" t="n">
+        <v>114131.7994019497</v>
+      </c>
+      <c r="D37" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-08-06
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1013,6 +1013,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>08/06/2025</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.0004301200000000026</v>
+      </c>
+      <c r="C38" t="n">
+        <v>116246.6288477627</v>
+      </c>
+      <c r="D38" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-08-10
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1029,6 +1029,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>08/10/2025</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.0004207599999999992</v>
+      </c>
+      <c r="C39" t="n">
+        <v>118832.5886491114</v>
+      </c>
+      <c r="D39" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-08-13
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1045,6 +1045,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>08/13/2025</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.0004084099999999979</v>
+      </c>
+      <c r="C40" t="n">
+        <v>122425.9934869378</v>
+      </c>
+      <c r="D40" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-08-17
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1061,6 +1061,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>08/17/2025</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.0004212500000000015</v>
+      </c>
+      <c r="C41" t="n">
+        <v>118694.3620178037</v>
+      </c>
+      <c r="D41" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-08-20
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1077,6 +1077,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>08/20/2025</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.0004368600000000007</v>
+      </c>
+      <c r="C42" t="n">
+        <v>114453.1428833034</v>
+      </c>
+      <c r="D42" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-08-24
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1093,6 +1093,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>08/24/2025</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.0004329499999999979</v>
+      </c>
+      <c r="C43" t="n">
+        <v>115486.7767640611</v>
+      </c>
+      <c r="D43" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-08-27
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1109,6 +1109,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>08/27/2025</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.0004426700000000026</v>
+      </c>
+      <c r="C44" t="n">
+        <v>112950.9566946025</v>
+      </c>
+      <c r="D44" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-08-31
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1125,6 +1125,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>08/31/2025</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.0004578099999999995</v>
+      </c>
+      <c r="C45" t="n">
+        <v>109215.613464101</v>
+      </c>
+      <c r="D45" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-09-03
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1141,6 +1141,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>09/03/2025</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.0004422799999999998</v>
+      </c>
+      <c r="C46" t="n">
+        <v>113050.5562087366</v>
+      </c>
+      <c r="D46" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-09-07
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1157,6 +1157,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>09/07/2025</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.0004494500000000005</v>
+      </c>
+      <c r="C47" t="n">
+        <v>111247.079764156</v>
+      </c>
+      <c r="D47" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-09-14
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1173,6 +1173,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>09/14/2025</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.0004291899999999994</v>
+      </c>
+      <c r="C48" t="n">
+        <v>116498.5204687902</v>
+      </c>
+      <c r="D48" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-09-21
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1189,6 +1189,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>09/21/2025</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.0004304399999999972</v>
+      </c>
+      <c r="C49" t="n">
+        <v>116160.2081590938</v>
+      </c>
+      <c r="D49" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-09-28
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1205,6 +1205,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>09/28/2025</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.0004548000000000017</v>
+      </c>
+      <c r="C50" t="n">
+        <v>109938.4344766926</v>
+      </c>
+      <c r="D50" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-10-05
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1221,6 +1221,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>10/05/2025</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.0003973100000000014</v>
+      </c>
+      <c r="C51" t="n">
+        <v>125846.3164783162</v>
+      </c>
+      <c r="D51" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-10-12
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1237,6 +1237,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.000445499999999998</v>
+      </c>
+      <c r="C52" t="n">
+        <v>112233.4455667794</v>
+      </c>
+      <c r="D52" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-10-19
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1253,6 +1253,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>10/19/2025</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.0004650000000000036</v>
+      </c>
+      <c r="C53" t="n">
+        <v>107526.8817204293</v>
+      </c>
+      <c r="D53" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-10-26
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1269,6 +1269,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>10/26/2025</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.000445999999999995</v>
+      </c>
+      <c r="C54" t="n">
+        <v>112107.6233183869</v>
+      </c>
+      <c r="D54" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-11-02
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1285,6 +1285,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>11/02/2025</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.0004510500000000014</v>
+      </c>
+      <c r="C55" t="n">
+        <v>110852.4553818863</v>
+      </c>
+      <c r="D55" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-11-09
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1301,6 +1301,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>11/09/2025</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.0004885600000000025</v>
+      </c>
+      <c r="C56" t="n">
+        <v>101318.1594891103</v>
+      </c>
+      <c r="D56" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-12-21
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1385,6 +1385,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>12/21/2025</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.0005591900000000011</v>
+      </c>
+      <c r="C62" t="n">
+        <v>88520.89629642859</v>
+      </c>
+      <c r="D62" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2025-12-28
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1401,6 +1401,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>12/28/2025</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.0005624099999999993</v>
+      </c>
+      <c r="C63" t="n">
+        <v>88014.08225316061</v>
+      </c>
+      <c r="D63" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2026-01-04
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1417,6 +1417,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>01/04/2026</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.0005391099999999989</v>
+      </c>
+      <c r="C64" t="n">
+        <v>91817.99632728033</v>
+      </c>
+      <c r="D64" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2026-01-11
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1433,6 +1433,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>01/11/2026</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.0005434200000000028</v>
+      </c>
+      <c r="C65" t="n">
+        <v>91089.76482278854</v>
+      </c>
+      <c r="D65" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2026-01-18
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1449,6 +1449,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>01/18/2026</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.0005181999999999964</v>
+      </c>
+      <c r="C66" t="n">
+        <v>95522.96410652323</v>
+      </c>
+      <c r="D66" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2026-01-25
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1465,6 +1465,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>01/25/2026</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.0005548899999999954</v>
+      </c>
+      <c r="C67" t="n">
+        <v>89206.86983005716</v>
+      </c>
+      <c r="D67" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2026-02-01
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1481,6 +1481,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>02/01/2026</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.0006264100000000078</v>
+      </c>
+      <c r="C68" t="n">
+        <v>79021.72698392329</v>
+      </c>
+      <c r="D68" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2026-02-08
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1497,6 +1497,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>02/08/2026</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.0007119599999999907</v>
+      </c>
+      <c r="C69" t="n">
+        <v>69526.37788639903</v>
+      </c>
+      <c r="D69" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2026-02-15
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1513,6 +1513,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>02/15/2026</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.0007009300000000024</v>
+      </c>
+      <c r="C70" t="n">
+        <v>70620.46138701416</v>
+      </c>
+      <c r="D70" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2026-02-22
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1529,6 +1529,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>02/22/2026</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.0007252900000000034</v>
+      </c>
+      <c r="C71" t="n">
+        <v>68248.56264390763</v>
+      </c>
+      <c r="D71" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update bitcoin_buys.xlsx after running on 2026-03-01
</commit_message>
<xml_diff>
--- a/data/bitcoin_buys.xlsx
+++ b/data/bitcoin_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1545,6 +1545,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0.0007296700000000017</v>
+      </c>
+      <c r="C72" t="n">
+        <v>67838.88607178572</v>
+      </c>
+      <c r="D72" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>